<commit_message>
B and C first iteration done
</commit_message>
<xml_diff>
--- a/Mechanical_Project/Inventor_project/Leg_press_parameters.xlsx
+++ b/Mechanical_Project/Inventor_project/Leg_press_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Caspe\Documents\Semester 8\Project\Anomaly_Detection\Mechanical_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Caspe\Documents\Semester 8\Project\Anomaly_Detection\Mechanical_Project\Inventor_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BDC1604-45D4-45AD-975A-601DB8C32838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B4715F2-A60E-4B7C-BE95-6629811A0541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3075" yWindow="3075" windowWidth="24945" windowHeight="11295" xr2:uid="{737F47E5-DFBE-4AFA-8C4F-443FB2B17703}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{737F47E5-DFBE-4AFA-8C4F-443FB2B17703}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="35">
   <si>
     <t>A_length</t>
   </si>
@@ -132,6 +132,15 @@
   </si>
   <si>
     <t>Gap between beam and hinge on each side</t>
+  </si>
+  <si>
+    <t>B_height</t>
+  </si>
+  <si>
+    <t>B_hinge_holes_spacing</t>
+  </si>
+  <si>
+    <t>A_B_spacing</t>
   </si>
 </sst>
 </file>
@@ -503,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4493E09F-6876-4379-A7D0-39BD24C74DF9}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="91" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="91" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -629,43 +638,43 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C11" t="s">
         <v>28</v>
-      </c>
-      <c r="D11" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B13">
-        <v>1200</v>
-      </c>
-      <c r="C13" t="s">
-        <v>28</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B14">
-        <v>50</v>
+        <v>700</v>
       </c>
       <c r="C14" t="s">
         <v>28</v>
@@ -673,10 +682,10 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="B15">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="C15" t="s">
         <v>28</v>
@@ -684,10 +693,10 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B16">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="C16" t="s">
         <v>28</v>
@@ -695,10 +704,10 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B17">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C17" t="s">
         <v>28</v>
@@ -706,7 +715,7 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B18">
         <v>40</v>
@@ -717,18 +726,21 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="C19" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="B20">
-        <v>300</v>
+        <v>50</v>
       </c>
       <c r="C20" t="s">
         <v>28</v>
@@ -736,10 +748,10 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B21">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C21" t="s">
         <v>28</v>
@@ -747,29 +759,29 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B22">
-        <v>400</v>
-      </c>
-      <c r="C22" t="s">
-        <v>28</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B23">
-        <v>0</v>
+        <v>400</v>
+      </c>
+      <c r="C23" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B24">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C24" t="s">
         <v>28</v>
@@ -777,10 +789,10 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B25">
-        <v>250</v>
+        <v>330</v>
       </c>
       <c r="C25" t="s">
         <v>28</v>
@@ -788,20 +800,50 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B26">
-        <v>2</v>
-      </c>
-      <c r="C26" t="s">
-        <v>28</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27">
+        <v>4</v>
+      </c>
+      <c r="C27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28">
+        <v>250</v>
+      </c>
+      <c r="C28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>22</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
         <v>21</v>
       </c>
-      <c r="B27">
+      <c r="B30">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
first time fully assembled
</commit_message>
<xml_diff>
--- a/Mechanical_Project/Inventor_project/Leg_press_parameters.xlsx
+++ b/Mechanical_Project/Inventor_project/Leg_press_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Caspe\Documents\Semester 8\Project\Anomaly_Detection\Mechanical_Project\Inventor_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94AFA9EF-BCB2-4FDC-9EB8-0C44E60A05F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75CC0E68-557A-46C2-99C3-03D583C75085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11295" xr2:uid="{737F47E5-DFBE-4AFA-8C4F-443FB2B17703}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{737F47E5-DFBE-4AFA-8C4F-443FB2B17703}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -182,8 +182,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -520,20 +521,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4493E09F-6876-4379-A7D0-39BD24C74DF9}">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="91" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:C32"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="91" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="17.75" customWidth="1"/>
+    <col min="2" max="2" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>24</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C1" t="s">
@@ -547,7 +549,7 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>1000</v>
       </c>
       <c r="C2" t="s">
@@ -558,7 +560,7 @@
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>50</v>
       </c>
       <c r="C3" t="s">
@@ -569,7 +571,7 @@
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>20</v>
       </c>
       <c r="C4" t="s">
@@ -580,7 +582,7 @@
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>40</v>
       </c>
       <c r="C5" t="s">
@@ -591,7 +593,7 @@
       <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>500</v>
       </c>
       <c r="C6" t="s">
@@ -602,7 +604,7 @@
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>10</v>
       </c>
       <c r="C7" t="s">
@@ -613,7 +615,7 @@
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>40</v>
       </c>
       <c r="C8" t="s">
@@ -624,7 +626,7 @@
       <c r="A9" t="s">
         <v>23</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>10</v>
       </c>
       <c r="C9" t="s">
@@ -635,7 +637,7 @@
       <c r="A10" t="s">
         <v>29</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>50</v>
       </c>
       <c r="C10" t="s">
@@ -646,7 +648,7 @@
       <c r="A11" t="s">
         <v>34</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>2</v>
       </c>
       <c r="C11" t="s">
@@ -657,7 +659,7 @@
       <c r="A12" t="s">
         <v>30</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
         <v>3</v>
       </c>
       <c r="C12" t="s">
@@ -671,7 +673,7 @@
       <c r="A13" t="s">
         <v>18</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
         <v>0</v>
       </c>
     </row>
@@ -679,7 +681,7 @@
       <c r="A14" t="s">
         <v>7</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1">
         <v>700</v>
       </c>
       <c r="C14" t="s">
@@ -690,7 +692,7 @@
       <c r="A15" t="s">
         <v>32</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="1">
         <v>50</v>
       </c>
       <c r="C15" t="s">
@@ -701,7 +703,7 @@
       <c r="A16" t="s">
         <v>8</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="1">
         <v>50</v>
       </c>
       <c r="C16" t="s">
@@ -712,7 +714,7 @@
       <c r="A17" t="s">
         <v>9</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="1">
         <v>20</v>
       </c>
       <c r="C17" t="s">
@@ -723,7 +725,7 @@
       <c r="A18" t="s">
         <v>10</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="1">
         <v>40</v>
       </c>
       <c r="C18" t="s">
@@ -734,7 +736,7 @@
       <c r="A19" t="s">
         <v>11</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="1">
         <v>10</v>
       </c>
       <c r="C19" t="s">
@@ -745,7 +747,7 @@
       <c r="A20" t="s">
         <v>33</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="1">
         <v>50</v>
       </c>
       <c r="C20" t="s">
@@ -756,7 +758,7 @@
       <c r="A21" t="s">
         <v>12</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="1">
         <v>40</v>
       </c>
       <c r="C21" t="s">
@@ -767,7 +769,7 @@
       <c r="A22" t="s">
         <v>19</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="1">
         <v>0</v>
       </c>
     </row>
@@ -775,7 +777,7 @@
       <c r="A23" t="s">
         <v>13</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="1">
         <v>400</v>
       </c>
       <c r="C23" t="s">
@@ -786,7 +788,7 @@
       <c r="A24" t="s">
         <v>14</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="1">
         <v>20</v>
       </c>
       <c r="C24" t="s">
@@ -797,7 +799,7 @@
       <c r="A25" t="s">
         <v>15</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="1">
         <v>330</v>
       </c>
       <c r="C25" t="s">
@@ -808,7 +810,7 @@
       <c r="A26" t="s">
         <v>20</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="1">
         <v>0</v>
       </c>
     </row>
@@ -816,8 +818,8 @@
       <c r="A27" t="s">
         <v>16</v>
       </c>
-      <c r="B27">
-        <v>4</v>
+      <c r="B27" s="1">
+        <v>3.35</v>
       </c>
       <c r="C27" t="s">
         <v>28</v>
@@ -827,7 +829,7 @@
       <c r="A28" t="s">
         <v>17</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="1">
         <v>250</v>
       </c>
       <c r="C28" t="s">
@@ -838,7 +840,7 @@
       <c r="A29" t="s">
         <v>22</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="1">
         <v>2</v>
       </c>
       <c r="C29" t="s">
@@ -849,7 +851,7 @@
       <c r="A30" t="s">
         <v>21</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="1">
         <v>0</v>
       </c>
     </row>
@@ -857,7 +859,7 @@
       <c r="A31" t="s">
         <v>35</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="1">
         <v>25</v>
       </c>
       <c r="C31" t="s">
@@ -868,7 +870,7 @@
       <c r="A32" t="s">
         <v>36</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="1">
         <v>21</v>
       </c>
       <c r="C32" t="s">

</xml_diff>